<commit_message>
[BI-2053] - updated test files
</commit_message>
<xml_diff>
--- a/src/files/TraitImport/test_traits_case_insensitivity.xlsx
+++ b/src/files/TraitImport/test_traits_case_insensitivity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hms243/IdeaProjects/taf/src/files/TraitImport/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mlm483/Source/taf/src/files/TraitImport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C739981B-39A1-CE44-8B01-86C98689F0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92D026C-8442-6D47-BFD6-D6D8BFC5AD32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="7060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4880" yWindow="500" windowWidth="37740" windowHeight="15140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Ordinal</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>ArchIVed</t>
-  </si>
-  <si>
-    <t>unit1</t>
   </si>
   <si>
     <t>unit2</t>
@@ -539,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -565,63 +562,63 @@
   <sheetData>
     <row r="1" spans="1:18" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="R1" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>6</v>
@@ -650,9 +647,7 @@
       <c r="L2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>15</v>
-      </c>
+      <c r="M2" s="8"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
@@ -660,12 +655,12 @@
         <v>3</v>
       </c>
       <c r="R2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>7</v>
@@ -695,7 +690,7 @@
       </c>
       <c r="L3" s="6"/>
       <c r="M3" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
@@ -709,9 +704,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -893,26 +891,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EFE1791-BEC8-419B-A7D8-F7EAC9E3F094}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7613A94-47D1-485D-A76D-D3A6CFAB63B4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="aa5be1c8-7296-4b7a-853c-c6802fcefdea"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -936,9 +923,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7613A94-47D1-485D-A76D-D3A6CFAB63B4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EFE1791-BEC8-419B-A7D8-F7EAC9E3F094}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="aa5be1c8-7296-4b7a-853c-c6802fcefdea"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update ontology sample files to match the latest version. Update entry from "Nominal' to "Numerical".
</commit_message>
<xml_diff>
--- a/src/files/TraitImport/test_traits_case_insensitivity.xlsx
+++ b/src/files/TraitImport/test_traits_case_insensitivity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hms243/IdeaProjects/taf/src/files/TraitImport/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\breedinginsight\cucumber\src\files\TraitImport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C739981B-39A1-CE44-8B01-86C98689F0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09F3149-9EC9-4CFD-8385-827CA9E6369D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="7060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-12" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
-  <si>
-    <t>Ordinal</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>method description</t>
   </si>
@@ -72,12 +69,6 @@
     <t>ArchIVed</t>
   </si>
   <si>
-    <t>unit1</t>
-  </si>
-  <si>
-    <t>unit2</t>
-  </si>
-  <si>
     <t>nAmE</t>
   </si>
   <si>
@@ -139,6 +130,12 @@
   </si>
   <si>
     <t>Germplasm AtTRIBUTE</t>
+  </si>
+  <si>
+    <t>Numerical</t>
+  </si>
+  <si>
+    <t>Index</t>
   </si>
 </sst>
 </file>
@@ -540,162 +537,162 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="B2" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>5</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="6" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
       <c r="Q2" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>9</v>
       </c>
       <c r="L3" s="6"/>
       <c r="M3" s="8" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
@@ -709,12 +706,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006D74C1D9EC8A1042A5EF45985DF3E9E4" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2000d971e1751a7db8d92151125d08a9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="aa5be1c8-7296-4b7a-853c-c6802fcefdea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a4a1f299a0d30015388c519f6ad441cc" ns3:_="">
     <xsd:import namespace="aa5be1c8-7296-4b7a-853c-c6802fcefdea"/>
@@ -892,7 +883,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -901,23 +892,13 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EFE1791-BEC8-419B-A7D8-F7EAC9E3F094}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="aa5be1c8-7296-4b7a-853c-c6802fcefdea"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{340A8394-9E0A-435F-BF61-25A36768AA02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -935,10 +916,26 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7613A94-47D1-485D-A76D-D3A6CFAB63B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EFE1791-BEC8-419B-A7D8-F7EAC9E3F094}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="aa5be1c8-7296-4b7a-853c-c6802fcefdea"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>